<commit_message>
WIP, about to replace current API with yfinance
</commit_message>
<xml_diff>
--- a/portfolio/portfolio.xlsx
+++ b/portfolio/portfolio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Desktop/portfolio-rebalancer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Desktop/portfolio-rebalancer/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02087001-0826-724D-80F8-0A4CB8DB31E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA2F34-BE19-BE45-9350-CFB1BADDA7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3AA64042-CA0E-3D46-B863-6D27FF0D38F9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Ticker</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>MSFT</t>
-  </si>
-  <si>
-    <t>Rebalance</t>
-  </si>
-  <si>
-    <t>Quarterly</t>
   </si>
 </sst>
 </file>
@@ -426,37 +420,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287746C2-F676-984D-9D9B-FFC7A3ECB6A4}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>0.3</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -464,7 +452,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -472,7 +460,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -480,7 +468,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -488,7 +476,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
WIP portfolio returns graph
</commit_message>
<xml_diff>
--- a/portfolio/portfolio.xlsx
+++ b/portfolio/portfolio.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Desktop/portfolio-rebalancer/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA2F34-BE19-BE45-9350-CFB1BADDA7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA3AC1C-11D1-4C40-8F14-C76729F01185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3AA64042-CA0E-3D46-B863-6D27FF0D38F9}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{3AA64042-CA0E-3D46-B863-6D27FF0D38F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Portfolio 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Portfolio 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Port3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Ticker</t>
   </si>
@@ -59,6 +61,39 @@
   </si>
   <si>
     <t>MSFT</t>
+  </si>
+  <si>
+    <t>GOOGL</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>LRCX</t>
+  </si>
+  <si>
+    <t>PYPL</t>
+  </si>
+  <si>
+    <t>YETI</t>
+  </si>
+  <si>
+    <t>QCOM</t>
+  </si>
+  <si>
+    <t>ETSY</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>CMG</t>
+  </si>
+  <si>
+    <t>SHOP</t>
+  </si>
+  <si>
+    <t>LOWE</t>
   </si>
 </sst>
 </file>
@@ -422,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287746C2-F676-984D-9D9B-FFC7A3ECB6A4}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,4 +522,190 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0006576A-AB23-3D47-8ADC-65996DA58AD5}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110E338C-E905-7949-9788-07F20DC14C40}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>